<commit_message>
adding univmon and opensketch code
</commit_message>
<xml_diff>
--- a/Analysis/Caida/Experiments/Analysis for Paper.xlsx
+++ b/Analysis/Caida/Experiments/Analysis for Paper.xlsx
@@ -572,11 +572,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223531544"/>
-        <c:axId val="223534288"/>
+        <c:axId val="520764360"/>
+        <c:axId val="520761224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223531544"/>
+        <c:axId val="520764360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -703,13 +703,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223534288"/>
+        <c:crossAx val="520761224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223534288"/>
+        <c:axId val="520761224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -757,6 +757,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -823,7 +824,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223531544"/>
+        <c:crossAx val="520764360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1319,11 +1320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223534680"/>
-        <c:axId val="223536248"/>
+        <c:axId val="520762008"/>
+        <c:axId val="520765928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223534680"/>
+        <c:axId val="520762008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -1450,13 +1451,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223536248"/>
+        <c:crossAx val="520765928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223536248"/>
+        <c:axId val="520765928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.30000000000000004"/>
@@ -1509,6 +1510,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1575,7 +1577,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223534680"/>
+        <c:crossAx val="520762008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.5000000000000005E-2"/>
@@ -2241,11 +2243,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223531152"/>
-        <c:axId val="223531936"/>
+        <c:axId val="520762400"/>
+        <c:axId val="520767496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223531152"/>
+        <c:axId val="520762400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4500"/>
@@ -2356,13 +2358,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223531936"/>
+        <c:crossAx val="520767496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223531936"/>
+        <c:axId val="520767496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2472,7 +2474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223531152"/>
+        <c:crossAx val="520762400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3132,11 +3134,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="140609896"/>
-        <c:axId val="140610288"/>
+        <c:axId val="520768672"/>
+        <c:axId val="520758872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="140609896"/>
+        <c:axId val="520768672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="75"/>
@@ -3254,13 +3256,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140610288"/>
+        <c:crossAx val="520758872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140610288"/>
+        <c:axId val="520758872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -3370,7 +3372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140609896"/>
+        <c:crossAx val="520768672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4008,11 +4010,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="140607936"/>
-        <c:axId val="140609112"/>
+        <c:axId val="520759264"/>
+        <c:axId val="520766320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="140607936"/>
+        <c:axId val="520759264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="75"/>
@@ -4123,13 +4125,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140609112"/>
+        <c:crossAx val="520766320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140609112"/>
+        <c:axId val="520766320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.55000000000000004"/>
@@ -4234,7 +4236,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140607936"/>
+        <c:crossAx val="520759264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4310,6 +4312,1836 @@
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Memory Trade Off </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>300 Heavy Hitters</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$19:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$H$19:$H$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.62705612142648703</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82028336011307201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91639445676976505</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95704467001149696</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98022757973271801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98881282192821096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99423301889114302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99581514244828895</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99788233908423796</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99827089962344195</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.998826347747513</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99886026953192297</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99853508028647797</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.998533684458492</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99855698810557603</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="511442424"/>
+        <c:axId val="511445952"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Space Saving</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="9525" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="103000"/>
+                            <a:lumMod val="102000"/>
+                            <a:tint val="94000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="110000"/>
+                            <a:lumMod val="100000"/>
+                            <a:shade val="100000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent1">
+                            <a:lumMod val="99000"/>
+                            <a:satMod val="120000"/>
+                            <a:shade val="78000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$2:$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>600</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>900</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1200</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1800</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2100</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2400</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2700</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3300</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3600</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>3900</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4200</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>4500</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$H$2:$H$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>0.466169366322221</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.60568518980799402</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.74259919695941501</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.90440476902035305</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.98329742387111896</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.99811242568182801</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.99893129502599998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.99908001926734802</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.99914303545121796</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.99917048439098599</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.99915274647614905</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.99919147806581099</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.99917695371968795</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.99921891294182097</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.99915436029238502</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Sample And Hold</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="9525" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent3">
+                            <a:satMod val="103000"/>
+                            <a:lumMod val="102000"/>
+                            <a:tint val="94000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent3">
+                            <a:satMod val="110000"/>
+                            <a:lumMod val="100000"/>
+                            <a:shade val="100000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="99000"/>
+                            <a:satMod val="120000"/>
+                            <a:shade val="78000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$36:$A$50</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>900</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1200</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1800</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2100</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2400</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2700</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3300</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3600</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3900</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>4200</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4500</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>4800</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$I$36:$I$50</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>0.51660826456741604</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.683872613995548</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.76234231187086599</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.80818269876485005</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.83980634908356999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.86308010013395697</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.87960022009781302</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.89296992113747597</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.90426769308660804</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.91358781586321502</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.92145537042180703</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.92825288394938399</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.93353929589795304</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.93803737443700996</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.94247019362278805</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="511442424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4500"/>
+          <c:min val="300"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (Number of flows tracked in the dataplane)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="511445952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="300"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="511445952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.45"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Weighted</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Fraction of TopK Accurately Reported</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="511442424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Memory Trade Off </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>300 Heavy Hitters</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$19:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$19:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.51561666666666595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.270666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13296666666666601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0686666666666606E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3326666666666602E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9529999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0290000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7166666666666599E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0433333333333302E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3433333333333301E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.31333333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2899999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.99E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0033333333333301E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.97E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="654475760"/>
+        <c:axId val="654481248"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Space Saving</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="9525" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="103000"/>
+                            <a:lumMod val="102000"/>
+                            <a:tint val="94000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="110000"/>
+                            <a:lumMod val="100000"/>
+                            <a:shade val="100000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent1">
+                            <a:lumMod val="99000"/>
+                            <a:satMod val="120000"/>
+                            <a:shade val="78000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$2:$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>600</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>900</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1200</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1800</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2100</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2400</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2700</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3300</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3600</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>3900</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4200</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>4500</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$H$2:$H$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>0.466169366322221</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.60568518980799402</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.74259919695941501</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.90440476902035305</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.98329742387111896</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.99811242568182801</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.99893129502599998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.99908001926734802</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.99914303545121796</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.99917048439098599</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.99915274647614905</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.99919147806581099</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.99917695371968795</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.99921891294182097</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.99915436029238502</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Sample And Hold</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="9525" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent3">
+                            <a:satMod val="103000"/>
+                            <a:lumMod val="102000"/>
+                            <a:tint val="94000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent3">
+                            <a:satMod val="110000"/>
+                            <a:lumMod val="100000"/>
+                            <a:shade val="100000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="99000"/>
+                            <a:satMod val="120000"/>
+                            <a:shade val="78000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$36:$A$50</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>900</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1200</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1800</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2100</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2400</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2700</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3300</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3600</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3900</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>4200</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4500</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>4800</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$I$36:$I$50</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>0.51660826456741604</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.683872613995548</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.76234231187086599</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.80818269876485005</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.83980634908356999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.86308010013395697</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.87960022009781302</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.89296992113747597</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.90426769308660804</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.91358781586321502</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.92145537042180703</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.92825288394938399</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.93353929589795304</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.93803737443700996</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.94247019362278805</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="654475760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4500"/>
+          <c:min val="300"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (Number of flows tracked in the dataplane)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654481248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="300"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="654481248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>False Negatives in </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>TopK  Reported</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654475760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -4513,6 +6345,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6504,6 +8416,964 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7053,16 +9923,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>70533</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>101013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>527039</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>116001</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542279</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>146481</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7140,6 +10010,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>198121</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7487,7 +10421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
@@ -8909,8 +11843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W170" workbookViewId="0">
-      <selection activeCell="AR120" sqref="AR120"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
backing up before changing hash functions
</commit_message>
<xml_diff>
--- a/Analysis/Caida/Experiments/Analysis for Paper.xlsx
+++ b/Analysis/Caida/Experiments/Analysis for Paper.xlsx
@@ -572,11 +572,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520764360"/>
-        <c:axId val="520761224"/>
+        <c:axId val="431393320"/>
+        <c:axId val="431400768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520764360"/>
+        <c:axId val="431393320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -703,13 +703,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520761224"/>
+        <c:crossAx val="431400768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520761224"/>
+        <c:axId val="431400768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -824,7 +824,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520764360"/>
+        <c:crossAx val="431393320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1320,11 +1320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520762008"/>
-        <c:axId val="520765928"/>
+        <c:axId val="431398416"/>
+        <c:axId val="431394888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520762008"/>
+        <c:axId val="431398416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -1451,13 +1451,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520765928"/>
+        <c:crossAx val="431394888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520765928"/>
+        <c:axId val="431394888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.30000000000000004"/>
@@ -1577,7 +1577,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520762008"/>
+        <c:crossAx val="431398416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.5000000000000005E-2"/>
@@ -2243,11 +2243,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520762400"/>
-        <c:axId val="520767496"/>
+        <c:axId val="431399592"/>
+        <c:axId val="431398024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520762400"/>
+        <c:axId val="431399592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4500"/>
@@ -2358,13 +2358,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520767496"/>
+        <c:crossAx val="431398024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520767496"/>
+        <c:axId val="431398024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2474,7 +2474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520762400"/>
+        <c:crossAx val="431399592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3134,11 +3134,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520768672"/>
-        <c:axId val="520758872"/>
+        <c:axId val="431395280"/>
+        <c:axId val="431395672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520768672"/>
+        <c:axId val="431395280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="75"/>
@@ -3256,13 +3256,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520758872"/>
+        <c:crossAx val="431395672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520758872"/>
+        <c:axId val="431395672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -3372,7 +3372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520768672"/>
+        <c:crossAx val="431395280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4010,11 +4010,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520759264"/>
-        <c:axId val="520766320"/>
+        <c:axId val="431396064"/>
+        <c:axId val="431396456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520759264"/>
+        <c:axId val="431396064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="75"/>
@@ -4064,7 +4064,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4125,13 +4124,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520766320"/>
+        <c:crossAx val="431396456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520766320"/>
+        <c:axId val="431396456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.55000000000000004"/>
@@ -4176,7 +4175,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4236,7 +4234,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520759264"/>
+        <c:crossAx val="431396064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4250,7 +4248,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4562,924 +4559,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="511442424"/>
-        <c:axId val="511445952"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:v>Space Saving</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="9525" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:gradFill rotWithShape="1">
-                      <a:gsLst>
-                        <a:gs pos="0">
-                          <a:schemeClr val="accent1">
-                            <a:satMod val="103000"/>
-                            <a:lumMod val="102000"/>
-                            <a:tint val="94000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="50000">
-                          <a:schemeClr val="accent1">
-                            <a:satMod val="110000"/>
-                            <a:lumMod val="100000"/>
-                            <a:shade val="100000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="100000">
-                          <a:schemeClr val="accent1">
-                            <a:lumMod val="99000"/>
-                            <a:satMod val="120000"/>
-                            <a:shade val="78000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                      </a:gsLst>
-                      <a:lin ang="5400000" scaled="0"/>
-                    </a:gradFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet2!$A$2:$A$16</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="15"/>
-                      <c:pt idx="0">
-                        <c:v>300</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>600</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>900</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1200</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>1500</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1800</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>2100</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>2400</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>2700</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>3000</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>3300</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>3600</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>3900</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>4200</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>4500</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet2!$H$2:$H$16</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="15"/>
-                      <c:pt idx="0">
-                        <c:v>0.466169366322221</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.60568518980799402</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.74259919695941501</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.90440476902035305</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.98329742387111896</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.99811242568182801</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>0.99893129502599998</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>0.99908001926734802</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>0.99914303545121796</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>0.99917048439098599</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>0.99915274647614905</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0.99919147806581099</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>0.99917695371968795</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>0.99921891294182097</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>0.99915436029238502</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:v>Sample And Hold</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="9525" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:gradFill rotWithShape="1">
-                      <a:gsLst>
-                        <a:gs pos="0">
-                          <a:schemeClr val="accent3">
-                            <a:satMod val="103000"/>
-                            <a:lumMod val="102000"/>
-                            <a:tint val="94000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="50000">
-                          <a:schemeClr val="accent3">
-                            <a:satMod val="110000"/>
-                            <a:lumMod val="100000"/>
-                            <a:shade val="100000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="100000">
-                          <a:schemeClr val="accent3">
-                            <a:lumMod val="99000"/>
-                            <a:satMod val="120000"/>
-                            <a:shade val="78000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                      </a:gsLst>
-                      <a:lin ang="5400000" scaled="0"/>
-                    </a:gradFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent3"/>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet2!$A$36:$A$50</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="15"/>
-                      <c:pt idx="0">
-                        <c:v>300</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>900</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1200</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1500</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>1800</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>2100</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>2400</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>2700</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>3000</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>3300</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>3600</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>3900</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>4200</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>4500</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>4800</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet2!$I$36:$I$50</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="15"/>
-                      <c:pt idx="0">
-                        <c:v>0.51660826456741604</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.683872613995548</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.76234231187086599</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.80818269876485005</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.83980634908356999</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.86308010013395697</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>0.87960022009781302</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>0.89296992113747597</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>0.90426769308660804</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>0.91358781586321502</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>0.92145537042180703</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0.92825288394938399</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>0.93353929589795304</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>0.93803737443700996</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>0.94247019362278805</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="511442424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="4500"/>
-          <c:min val="300"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx2"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Memory</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (Number of flows tracked in the dataplane)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="511445952"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="300"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="511445952"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0.45"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx2"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Weighted</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Fraction of TopK Accurately Reported</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="40000"/>
-                <a:lumOff val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="511442424"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx2">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Accuracy</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs Memory Trade Off </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>300 Heavy Hitters</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="9525" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent2">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$A$19:$A$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2100</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3300</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3900</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$E$19:$E$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0.51561666666666595</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.270666666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.13296666666666601</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.0686666666666606E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.3326666666666602E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.9529999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0290000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.7166666666666599E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.0433333333333302E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.3433333333333301E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.31333333333333E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.2899999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.99E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.0033333333333301E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.97E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="654475760"/>
-        <c:axId val="654481248"/>
+        <c:axId val="434934760"/>
+        <c:axId val="434938288"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -5842,7 +4923,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="654475760"/>
+        <c:axId val="434934760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4500"/>
@@ -5953,13 +5034,929 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="654481248"/>
+        <c:crossAx val="434938288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="654481248"/>
+        <c:axId val="434938288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.45"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Weighted</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Fraction of TopK Accurately Reported</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="434934760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Memory Trade Off </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>300 Heavy Hitters</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$19:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$19:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.51561666666666595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.270666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13296666666666601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0686666666666606E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3326666666666602E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9529999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0290000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7166666666666599E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0433333333333302E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3433333333333301E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.31333333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2899999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.99E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0033333333333301E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.97E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="434936720"/>
+        <c:axId val="434937112"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Space Saving</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="9525" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="103000"/>
+                            <a:lumMod val="102000"/>
+                            <a:tint val="94000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="110000"/>
+                            <a:lumMod val="100000"/>
+                            <a:shade val="100000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent1">
+                            <a:lumMod val="99000"/>
+                            <a:satMod val="120000"/>
+                            <a:shade val="78000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$2:$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>600</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>900</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1200</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1800</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2100</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2400</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2700</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3300</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3600</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>3900</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4200</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>4500</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$H$2:$H$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>0.466169366322221</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.60568518980799402</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.74259919695941501</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.90440476902035305</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.98329742387111896</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.99811242568182801</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.99893129502599998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.99908001926734802</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.99914303545121796</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.99917048439098599</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.99915274647614905</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.99919147806581099</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.99917695371968795</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.99921891294182097</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.99915436029238502</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Sample And Hold</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="9525" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent3">
+                            <a:satMod val="103000"/>
+                            <a:lumMod val="102000"/>
+                            <a:tint val="94000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent3">
+                            <a:satMod val="110000"/>
+                            <a:lumMod val="100000"/>
+                            <a:shade val="100000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="99000"/>
+                            <a:satMod val="120000"/>
+                            <a:shade val="78000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$36:$A$50</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>900</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1200</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1800</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2100</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2400</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2700</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3300</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3600</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3900</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>4200</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4500</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>4800</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$I$36:$I$50</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>0.51660826456741604</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.683872613995548</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.76234231187086599</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.80818269876485005</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.83980634908356999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.86308010013395697</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.87960022009781302</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.89296992113747597</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.90426769308660804</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.91358781586321502</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.92145537042180703</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.92825288394938399</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.93353929589795304</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.93803737443700996</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.94247019362278805</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="434936720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4500"/>
+          <c:min val="300"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (Number of flows tracked in the dataplane)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="434937112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="300"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="434937112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6067,7 +6064,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="654475760"/>
+        <c:crossAx val="434936720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9923,16 +9920,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>101013</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>17193</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>542279</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>146481</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>458459</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>62661</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10017,16 +10014,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>434341</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>198121</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>251461</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10421,7 +10418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
@@ -11843,8 +11840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="M64" sqref="M64"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>